<commit_message>
Gateway Worked on Modem SMS new SIM Modul etc..
</commit_message>
<xml_diff>
--- a/Gateway/doc/Gateway_Dataformat.xlsx
+++ b/Gateway/doc/Gateway_Dataformat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raffael\GitHub\P6_Software_local\my_projects\NRD\Gateway\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3939DA6B-FD8A-4795-986D-C0540DDB1AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645D8027-9E2A-4F10-9EC8-FEF175096E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{39BEC552-0458-4A70-9E23-C987F9B861A4}"/>
+    <workbookView xWindow="0" yWindow="3870" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{39BEC552-0458-4A70-9E23-C987F9B861A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Mobile" sheetId="1" r:id="rId1"/>
@@ -783,7 +783,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,7 +1113,7 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,7 +1988,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,15 +2033,15 @@
         <v>0.5</v>
       </c>
       <c r="E2">
-        <f>(C2-B2)/D2</f>
+        <f t="shared" ref="E2:E9" si="0">(C2-B2)/D2</f>
         <v>250</v>
       </c>
       <c r="F2">
-        <f>ROUNDUP(LOG(E2,2),0)</f>
+        <f t="shared" ref="F2:F9" si="1">ROUNDUP(LOG(E2,2),0)</f>
         <v>8</v>
       </c>
       <c r="G2">
-        <f>MOD(LOG(E2,2),1)</f>
+        <f t="shared" ref="G2:G9" si="2">MOD(LOG(E2,2),1)</f>
         <v>0.96578428466208699</v>
       </c>
     </row>
@@ -2060,15 +2060,15 @@
         <v>0.1</v>
       </c>
       <c r="E3">
-        <f>(C3-B3)/D3</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="F3">
-        <f>ROUNDUP(LOG(E3,2),0)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G3">
-        <f>MOD(LOG(E3,2),1)</f>
+        <f t="shared" si="2"/>
         <v>0.96578428466208699</v>
       </c>
     </row>
@@ -2086,15 +2086,15 @@
         <v>10</v>
       </c>
       <c r="E4">
-        <f>(C4-B4)/D4</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="F4">
-        <f>ROUNDUP(LOG(E4,2),0)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G4">
-        <f>MOD(LOG(E4,2),1)</f>
+        <f t="shared" si="2"/>
         <v>0.96578428466208699</v>
       </c>
     </row>
@@ -2112,15 +2112,15 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <f>(C5-B5)/D5</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="F5">
-        <f>ROUNDUP(LOG(E5,2),0)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G5">
-        <f>MOD(LOG(E5,2),1)</f>
+        <f t="shared" si="2"/>
         <v>0.96578428466208699</v>
       </c>
     </row>
@@ -2138,15 +2138,15 @@
         <v>0.1</v>
       </c>
       <c r="E6">
-        <f>(C6-B6)/D6</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="F6">
-        <f>ROUNDUP(LOG(E6,2),0)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G6">
-        <f>MOD(LOG(E6,2),1)</f>
+        <f t="shared" si="2"/>
         <v>0.96578428466208699</v>
       </c>
     </row>
@@ -2164,15 +2164,15 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <f>(C7-B7)/D7</f>
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
       <c r="F7">
-        <f>ROUNDUP(LOG(E7,2),0)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G7">
-        <f>MOD(LOG(E7,2),1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2190,15 +2190,15 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <f>(C8-B8)/D8</f>
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
       <c r="F8">
-        <f>ROUNDUP(LOG(E8,2),0)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G8">
-        <f>MOD(LOG(E8,2),1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2216,15 +2216,15 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <f>(C9-B9)/D9</f>
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
       <c r="F9">
-        <f>ROUNDUP(LOG(E9,2),0)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G9">
-        <f>MOD(LOG(E9,2),1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>